<commit_message>
add JOP and update formatting
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262A3380-F132-274F-8FD3-D86FA74B4719}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B023B5-F3D4-574C-B3E8-8E8EC57EF02D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>article_wordlimit</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>https://ajps.org/guidelines-for-manuscripts/manuscript-preparation/</t>
+  </si>
+  <si>
+    <t>12,000 words</t>
+  </si>
+  <si>
+    <t>10,000 words</t>
+  </si>
+  <si>
+    <t>4,000 words</t>
+  </si>
+  <si>
+    <t>JOURNAL OF POLITICS</t>
+  </si>
+  <si>
+    <t>https://www.journals.uchicago.edu/journals/jop/instruct</t>
+  </si>
+  <si>
+    <t>35 pages</t>
+  </si>
+  <si>
+    <t>10 pages</t>
   </si>
 </sst>
 </file>
@@ -414,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,11 +470,11 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>12000</v>
-      </c>
-      <c r="C2">
-        <v>4000</v>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -466,13 +487,30 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>10000</v>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3">
+        <v>20190903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
         <v>20190903</v>
       </c>
     </row>
@@ -480,6 +518,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{F2260C3F-4BE2-7F41-B331-8F6C5BA48B38}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{99EAA63A-BADD-544B-B9EC-CD4DE4D7D64F}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{719B026B-6B4F-0E4F-A567-5C3ED7496B9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix IJPP and add two journals
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16A2F8C-EC31-574D-BF3E-15E4AA427750}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBCDAE7-23D6-3740-93B2-49A28894979D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="295">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -898,6 +898,18 @@
   </si>
   <si>
     <t>https://academic.oup.com/jrs/pages/General_Instructions</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/joc/pages/General_Instructions#Submission%20Guidelines</t>
+  </si>
+  <si>
+    <t>JOURNAL OF COMMUNICATION</t>
+  </si>
+  <si>
+    <t>https://us.sagepub.com/en-us/nam/journal/communication-research#submission-guidelines</t>
+  </si>
+  <si>
+    <t>COMMUNICATION RESEARCH</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,6 +3253,34 @@
       </c>
       <c r="F129">
         <v>20190908</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F130">
+        <v>20190918</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>294</v>
+      </c>
+      <c r="B131" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F131">
+        <v>20190918</v>
       </c>
     </row>
   </sheetData>
@@ -3373,6 +3413,8 @@
     <hyperlink ref="E127" r:id="rId126" location="words" xr:uid="{AE11DD0F-E0C6-E44E-B52F-EC27F4687C95}"/>
     <hyperlink ref="E128" r:id="rId127" location="words" xr:uid="{23DE4BAA-D9C5-2B4C-9104-26BABBD442FA}"/>
     <hyperlink ref="E129" r:id="rId128" xr:uid="{5453FAE7-1BD2-5D4F-BCC7-2157562E236C}"/>
+    <hyperlink ref="E130" r:id="rId129" location="Submission%20Guidelines" xr:uid="{FABF0571-A4D5-9940-820E-57F16419C70E}"/>
+    <hyperlink ref="E131" r:id="rId130" location="submission-guidelines" xr:uid="{4725D78F-A57F-FE4C-8C42-119485F303DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Research & Politics'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBCDAE7-23D6-3740-93B2-49A28894979D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C6019B-F69F-1E4B-BFEF-207EF54D1DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="297">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -910,6 +910,12 @@
   </si>
   <si>
     <t>COMMUNICATION RESEARCH</t>
+  </si>
+  <si>
+    <t>Research &amp; Politics</t>
+  </si>
+  <si>
+    <t>https://us.sagepub.com/en-us/nam/journal/research-politics#submission-guidelines</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3281,6 +3287,23 @@
       </c>
       <c r="F131">
         <v>20190918</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>295</v>
+      </c>
+      <c r="B132" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" t="s">
+        <v>115</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F132">
+        <v>20191005</v>
       </c>
     </row>
   </sheetData>
@@ -3415,6 +3438,7 @@
     <hyperlink ref="E129" r:id="rId128" xr:uid="{5453FAE7-1BD2-5D4F-BCC7-2157562E236C}"/>
     <hyperlink ref="E130" r:id="rId129" location="Submission%20Guidelines" xr:uid="{FABF0571-A4D5-9940-820E-57F16419C70E}"/>
     <hyperlink ref="E131" r:id="rId130" location="submission-guidelines" xr:uid="{4725D78F-A57F-FE4C-8C42-119485F303DA}"/>
+    <hyperlink ref="E132" r:id="rId131" location="submission-guidelines" xr:uid="{57DDE689-B0DB-E246-8E7D-558AA3C5D718}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Frontiers in Political Science'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C6019B-F69F-1E4B-BFEF-207EF54D1DDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEEC3DA-DF11-9C41-88A8-EF0E57AD02A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="299">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -916,6 +916,12 @@
   </si>
   <si>
     <t>https://us.sagepub.com/en-us/nam/journal/research-politics#submission-guidelines</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/journals/political-science#author-guidelines</t>
+  </si>
+  <si>
+    <t>Frontiers in Political Science</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3304,6 +3310,26 @@
       </c>
       <c r="F132">
         <v>20191005</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>298</v>
+      </c>
+      <c r="B133" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" t="s">
+        <v>7</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F133">
+        <v>20191206</v>
       </c>
     </row>
   </sheetData>
@@ -3439,6 +3465,7 @@
     <hyperlink ref="E130" r:id="rId129" location="Submission%20Guidelines" xr:uid="{FABF0571-A4D5-9940-820E-57F16419C70E}"/>
     <hyperlink ref="E131" r:id="rId130" location="submission-guidelines" xr:uid="{4725D78F-A57F-FE4C-8C42-119485F303DA}"/>
     <hyperlink ref="E132" r:id="rId131" location="submission-guidelines" xr:uid="{57DDE689-B0DB-E246-8E7D-558AA3C5D718}"/>
+    <hyperlink ref="E133" r:id="rId132" location="author-guidelines" xr:uid="{3B4D866F-35E0-3F4C-81D8-61396E370F59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'Politics and The Life Sciences'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387DA9D7-336D-5A46-A3C8-FBF0E9F89B30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572358B9-4C73-6648-BD8C-5C7BADEF773A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="303">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -928,6 +928,12 @@
   </si>
   <si>
     <t>https://journals.sagepub.com/author-instructions/POL</t>
+  </si>
+  <si>
+    <t>Politics and the Life Sciences</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/politics-and-the-life-sciences/information/instructions-contributors</t>
   </si>
 </sst>
 </file>
@@ -1290,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3350,6 +3356,26 @@
       </c>
       <c r="F134">
         <v>20191208</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>301</v>
+      </c>
+      <c r="B135" t="s">
+        <v>67</v>
+      </c>
+      <c r="C135" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F135">
+        <v>20191227</v>
       </c>
     </row>
   </sheetData>
@@ -3487,6 +3513,7 @@
     <hyperlink ref="E132" r:id="rId131" location="submission-guidelines" xr:uid="{57DDE689-B0DB-E246-8E7D-558AA3C5D718}"/>
     <hyperlink ref="E133" r:id="rId132" location="author-guidelines" xr:uid="{3B4D866F-35E0-3F4C-81D8-61396E370F59}"/>
     <hyperlink ref="E134" r:id="rId133" xr:uid="{D9F6D1C2-1F90-5B4E-9CBC-B40F8ACC2B5D}"/>
+    <hyperlink ref="E135" r:id="rId134" xr:uid="{D6900322-5974-6D4F-B504-EE9B5F10B965}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'European Policy Analysis'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572358B9-4C73-6648-BD8C-5C7BADEF773A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736ADB0A-3913-494C-9D72-72356E6163E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="305">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -934,6 +934,12 @@
   </si>
   <si>
     <t>https://www.cambridge.org/core/journals/politics-and-the-life-sciences/information/instructions-contributors</t>
+  </si>
+  <si>
+    <t>European Policy Analysis</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/page/journal/23806567/homepage/forauthors.html</t>
   </si>
 </sst>
 </file>
@@ -1296,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3376,6 +3382,20 @@
       </c>
       <c r="F135">
         <v>20191227</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>303</v>
+      </c>
+      <c r="B136" t="s">
+        <v>15</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F136">
+        <v>20200225</v>
       </c>
     </row>
   </sheetData>
@@ -3514,6 +3534,7 @@
     <hyperlink ref="E133" r:id="rId132" location="author-guidelines" xr:uid="{3B4D866F-35E0-3F4C-81D8-61396E370F59}"/>
     <hyperlink ref="E134" r:id="rId133" xr:uid="{D9F6D1C2-1F90-5B4E-9CBC-B40F8ACC2B5D}"/>
     <hyperlink ref="E135" r:id="rId134" xr:uid="{D6900322-5974-6D4F-B504-EE9B5F10B965}"/>
+    <hyperlink ref="E136" r:id="rId135" xr:uid="{54D6C659-41FF-8849-A5F2-F9398C5C64A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'European Sociological Review'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736ADB0A-3913-494C-9D72-72356E6163E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EB198C-F164-F24C-98BA-56A2AFD074FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="307">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -940,6 +940,12 @@
   </si>
   <si>
     <t>https://onlinelibrary.wiley.com/page/journal/23806567/homepage/forauthors.html</t>
+  </si>
+  <si>
+    <t>EUROPEAN SOCIOLOGICAL REVIEW</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/esr/pages/General_Instructions</t>
   </si>
 </sst>
 </file>
@@ -1302,9 +1308,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
       <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
@@ -3396,6 +3402,20 @@
       </c>
       <c r="F136">
         <v>20200225</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>305</v>
+      </c>
+      <c r="B137" t="s">
+        <v>15</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F137">
+        <v>20200416</v>
       </c>
     </row>
   </sheetData>
@@ -3535,6 +3555,7 @@
     <hyperlink ref="E134" r:id="rId133" xr:uid="{D9F6D1C2-1F90-5B4E-9CBC-B40F8ACC2B5D}"/>
     <hyperlink ref="E135" r:id="rId134" xr:uid="{D6900322-5974-6D4F-B504-EE9B5F10B965}"/>
     <hyperlink ref="E136" r:id="rId135" xr:uid="{54D6C659-41FF-8849-A5F2-F9398C5C64A2}"/>
+    <hyperlink ref="E137" r:id="rId136" xr:uid="{55416B20-60A2-0741-B9E9-312DD4DDCA42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 'Social Science Journal'
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Dropbox/web/GitHub/poliscijournals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikgahnerlarsen/Documents/poliscijournals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EB198C-F164-F24C-98BA-56A2AFD074FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C9E40-50FF-9A4B-97AA-FFBDB37976CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="17100" xr2:uid="{51A4E432-F3E5-8944-A4F2-8D984DDB9D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="307">
   <si>
     <t>https://www.cambridge.org/core/journals/american-political-science-review/information/instructions-contributors</t>
   </si>
@@ -720,9 +720,6 @@
     <t>SOCIAL SCIENCE JOURNAL</t>
   </si>
   <si>
-    <t>https://www.elsevier.com/journals/the-social-science-journal/0362-3319/guide-for-authors</t>
-  </si>
-  <si>
     <t>British Journal of Politics &amp; International Relations</t>
   </si>
   <si>
@@ -946,6 +943,9 @@
   </si>
   <si>
     <t>https://academic.oup.com/esr/pages/General_Instructions</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/action/authorSubmission?show=instructions&amp;journalCode=ussj20</t>
   </si>
 </sst>
 </file>
@@ -995,7 +995,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1012,7 +1012,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2807FA76-560D-4145-BA30-BBF62FA6055B}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2857,25 +2857,22 @@
       <c r="B100" t="s">
         <v>120</v>
       </c>
-      <c r="C100" t="s">
-        <v>13</v>
-      </c>
       <c r="E100" s="1" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F100">
-        <v>20190907</v>
+        <v>20210731</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B101" t="s">
         <v>15</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F101">
         <v>20190907</v>
@@ -2883,13 +2880,13 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F102">
         <v>20190907</v>
@@ -2897,13 +2894,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B103" t="s">
         <v>208</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F103">
         <v>20190908</v>
@@ -2911,7 +2908,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B104" t="s">
         <v>15</v>
@@ -2920,7 +2917,7 @@
         <v>17</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F104">
         <v>20190908</v>
@@ -2928,13 +2925,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F105">
         <v>20190908</v>
@@ -2942,13 +2939,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F106">
         <v>20190908</v>
@@ -2956,13 +2953,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F107">
         <v>20190908</v>
@@ -2970,7 +2967,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B108" t="s">
         <v>67</v>
@@ -2979,7 +2976,7 @@
         <v>8</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F108">
         <v>20190908</v>
@@ -2987,13 +2984,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>247</v>
+      </c>
+      <c r="B109" t="s">
         <v>248</v>
       </c>
-      <c r="B109" t="s">
+      <c r="E109" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="F109">
         <v>20190908</v>
@@ -3001,13 +2998,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B110" t="s">
         <v>8</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F110">
         <v>20190908</v>
@@ -3015,13 +3012,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B111" t="s">
         <v>15</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F111">
         <v>20190908</v>
@@ -3029,13 +3026,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F112">
         <v>20190908</v>
@@ -3043,7 +3040,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B113" t="s">
         <v>45</v>
@@ -3052,7 +3049,7 @@
         <v>9</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F113">
         <v>20190908</v>
@@ -3060,13 +3057,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B114" t="s">
         <v>150</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F114">
         <v>20190908</v>
@@ -3074,13 +3071,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F115">
         <v>20190908</v>
@@ -3088,7 +3085,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B116" t="s">
         <v>71</v>
@@ -3097,7 +3094,7 @@
         <v>42</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F116">
         <v>20190908</v>
@@ -3105,13 +3102,13 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B117" t="s">
         <v>208</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F117">
         <v>20190908</v>
@@ -3119,13 +3116,13 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B118" t="s">
         <v>15</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F118">
         <v>20190908</v>
@@ -3133,13 +3130,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B119" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F119">
         <v>20190908</v>
@@ -3147,7 +3144,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B120" t="s">
         <v>71</v>
@@ -3156,7 +3153,7 @@
         <v>42</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F120">
         <v>20190908</v>
@@ -3164,7 +3161,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B121" t="s">
         <v>45</v>
@@ -3173,7 +3170,7 @@
         <v>17</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F121">
         <v>20190908</v>
@@ -3181,13 +3178,13 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B122" t="s">
         <v>15</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F122">
         <v>20190908</v>
@@ -3195,13 +3192,13 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F123">
         <v>20190908</v>
@@ -3209,13 +3206,13 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B124" t="s">
         <v>15</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F124">
         <v>20190908</v>
@@ -3223,13 +3220,13 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F125">
         <v>20190908</v>
@@ -3237,13 +3234,13 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F126">
         <v>20190908</v>
@@ -3251,13 +3248,13 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B127" t="s">
         <v>15</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F127">
         <v>20190908</v>
@@ -3265,13 +3262,13 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B128" t="s">
         <v>17</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F128">
         <v>20190908</v>
@@ -3279,13 +3276,13 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B129" t="s">
         <v>15</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F129">
         <v>20190908</v>
@@ -3293,13 +3290,13 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B130" t="s">
         <v>12</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F130">
         <v>20190918</v>
@@ -3307,13 +3304,13 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B131" t="s">
         <v>12</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F131">
         <v>20190918</v>
@@ -3321,7 +3318,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B132" t="s">
         <v>9</v>
@@ -3330,7 +3327,7 @@
         <v>115</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F132">
         <v>20191005</v>
@@ -3338,7 +3335,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
@@ -3350,7 +3347,7 @@
         <v>7</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F133">
         <v>20191206</v>
@@ -3358,13 +3355,13 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B134" t="s">
         <v>15</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F134">
         <v>20191208</v>
@@ -3372,7 +3369,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B135" t="s">
         <v>67</v>
@@ -3384,7 +3381,7 @@
         <v>8</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F135">
         <v>20191227</v>
@@ -3392,13 +3389,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B136" t="s">
         <v>15</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F136">
         <v>20200225</v>
@@ -3406,13 +3403,13 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B137" t="s">
         <v>15</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F137">
         <v>20200416</v>

</xml_diff>